<commit_message>
other simulations and python code to plot false positive vs false negative
</commit_message>
<xml_diff>
--- a/code/Analysis.xlsx
+++ b/code/Analysis.xlsx
@@ -4,19 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>True Positive</t>
   </si>
@@ -61,6 +59,30 @@
   </si>
   <si>
     <t>C1=2.4</t>
+  </si>
+  <si>
+    <t>C1=2.6</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>C1=2.8</t>
+  </si>
+  <si>
+    <t>C2=0.2</t>
+  </si>
+  <si>
+    <t>C2=0.4</t>
+  </si>
+  <si>
+    <t>C2=0.6</t>
+  </si>
+  <si>
+    <t>C2=0.8</t>
+  </si>
+  <si>
+    <t>C2=1.0</t>
   </si>
 </sst>
 </file>
@@ -399,255 +421,375 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
       </c>
       <c r="B2">
         <v>30249</v>
       </c>
       <c r="C2">
+        <v>2255</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>107801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
         <v>8061</v>
-      </c>
-      <c r="D2">
-        <v>9889</v>
-      </c>
-      <c r="E2">
-        <v>12096</v>
-      </c>
-      <c r="F2">
-        <v>15563</v>
-      </c>
-      <c r="G2">
-        <v>22945</v>
-      </c>
-      <c r="H2">
-        <v>30249</v>
-      </c>
-      <c r="I2">
-        <v>29238</v>
-      </c>
-      <c r="J2">
-        <v>30103</v>
-      </c>
-      <c r="K2">
-        <v>29906</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2255</v>
       </c>
       <c r="C3">
         <v>936</v>
       </c>
       <c r="D3">
+        <v>1319</v>
+      </c>
+      <c r="E3">
+        <v>22188</v>
+      </c>
+      <c r="F3">
+        <v>51341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>9889</v>
+      </c>
+      <c r="C4">
         <v>1018</v>
-      </c>
-      <c r="E3">
-        <v>1155</v>
-      </c>
-      <c r="F3">
-        <v>1333</v>
-      </c>
-      <c r="G3">
-        <v>1762</v>
-      </c>
-      <c r="H3">
-        <v>2255</v>
-      </c>
-      <c r="I3">
-        <v>1664</v>
-      </c>
-      <c r="J3">
-        <v>2106</v>
-      </c>
-      <c r="K3">
-        <v>1969</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>1319</v>
       </c>
       <c r="D4">
         <v>1237</v>
       </c>
       <c r="E4">
+        <v>20360</v>
+      </c>
+      <c r="F4">
+        <v>59792</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>12096</v>
+      </c>
+      <c r="C5">
+        <v>1155</v>
+      </c>
+      <c r="D5">
         <v>1100</v>
-      </c>
-      <c r="F4">
-        <v>922</v>
-      </c>
-      <c r="G4">
-        <v>493</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>591</v>
-      </c>
-      <c r="J4">
-        <v>149</v>
-      </c>
-      <c r="K4">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>22188</v>
-      </c>
-      <c r="D5">
-        <v>20360</v>
       </c>
       <c r="E5">
         <v>18153</v>
       </c>
       <c r="F5">
+        <v>69422</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>15563</v>
+      </c>
+      <c r="C6">
+        <v>1333</v>
+      </c>
+      <c r="D6">
+        <v>922</v>
+      </c>
+      <c r="E6">
         <v>14686</v>
-      </c>
-      <c r="G5">
-        <v>7304</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>1011</v>
-      </c>
-      <c r="J5">
-        <v>146</v>
-      </c>
-      <c r="K5">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>107801</v>
-      </c>
-      <c r="C6">
-        <v>51341</v>
-      </c>
-      <c r="D6">
-        <v>59792</v>
-      </c>
-      <c r="E6">
-        <v>69422</v>
       </c>
       <c r="F6">
         <v>80659</v>
       </c>
-      <c r="G6">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>22945</v>
+      </c>
+      <c r="C7">
+        <v>1762</v>
+      </c>
+      <c r="D7">
+        <v>493</v>
+      </c>
+      <c r="E7">
+        <v>7304</v>
+      </c>
+      <c r="F7">
         <v>94912</v>
       </c>
-      <c r="H6">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>30249</v>
+      </c>
+      <c r="C8">
+        <v>2255</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>126348</v>
       </c>
-      <c r="I6">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>29238</v>
+      </c>
+      <c r="C9">
+        <v>1664</v>
+      </c>
+      <c r="D9">
+        <v>591</v>
+      </c>
+      <c r="E9">
+        <v>1011</v>
+      </c>
+      <c r="F9">
         <v>93756</v>
       </c>
-      <c r="J6">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>30103</v>
+      </c>
+      <c r="C10">
+        <v>2106</v>
+      </c>
+      <c r="D10">
+        <v>149</v>
+      </c>
+      <c r="E10">
+        <v>146</v>
+      </c>
+      <c r="F10">
         <v>104797</v>
       </c>
-      <c r="K6">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>29906</v>
+      </c>
+      <c r="C11">
+        <v>1969</v>
+      </c>
+      <c r="D11">
+        <v>286</v>
+      </c>
+      <c r="E11">
+        <v>343</v>
+      </c>
+      <c r="F11">
         <v>101971</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>29689</v>
+      </c>
+      <c r="C12">
+        <v>1858</v>
+      </c>
+      <c r="D12">
+        <v>397</v>
+      </c>
+      <c r="E12">
+        <v>560</v>
+      </c>
+      <c r="F12">
+        <v>99316</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>29466</v>
+      </c>
+      <c r="C13">
+        <v>1750</v>
+      </c>
+      <c r="D13">
+        <v>505</v>
+      </c>
+      <c r="E13">
+        <v>783</v>
+      </c>
+      <c r="F13">
+        <v>96681</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>26000</v>
+      </c>
+      <c r="C14">
+        <v>1766</v>
+      </c>
+      <c r="D14">
+        <v>489</v>
+      </c>
+      <c r="E14">
+        <v>4249</v>
+      </c>
+      <c r="F14">
+        <v>88576</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>22501</v>
+      </c>
+      <c r="C15">
+        <v>1423</v>
+      </c>
+      <c r="D15">
+        <v>832</v>
+      </c>
+      <c r="E15">
+        <v>7748</v>
+      </c>
+      <c r="F15">
+        <v>74544</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>18576</v>
+      </c>
+      <c r="C16">
+        <v>947</v>
+      </c>
+      <c r="D16">
+        <v>1308</v>
+      </c>
+      <c r="E16">
+        <v>11673</v>
+      </c>
+      <c r="F16">
+        <v>58914</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>14248</v>
+      </c>
+      <c r="C17">
+        <v>568</v>
+      </c>
+      <c r="D17">
+        <v>1687</v>
+      </c>
+      <c r="E17">
+        <v>16001</v>
+      </c>
+      <c r="F17">
+        <v>42789</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>10283</v>
+      </c>
+      <c r="C18">
+        <v>358</v>
+      </c>
+      <c r="D18">
+        <v>1897</v>
+      </c>
+      <c r="E18">
+        <v>19966</v>
+      </c>
+      <c r="F18">
+        <v>29145</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>